<commit_message>
Modify Variables doc to account for changes
</commit_message>
<xml_diff>
--- a/group_g_assignments/data/clean/Variables.xlsx
+++ b/group_g_assignments/data/clean/Variables.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\T450s\Desktop\programming\git\ba_da1\data\clean\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\T450s\Desktop\programming\git\ba_da1\group_g_assignments\data\clean\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B73C7EAD-6148-41FC-B6E0-604387CB8CE6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76895433-BA48-41FB-A908-DE9332A1EFC2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25170" yWindow="-1590" windowWidth="21600" windowHeight="11385" xr2:uid="{BF0F722A-D5EF-4B24-BABF-EC1503209A71}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{BF0F722A-D5EF-4B24-BABF-EC1503209A71}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="35">
   <si>
     <t>Variable</t>
   </si>
@@ -72,9 +72,6 @@
     <t>chr</t>
   </si>
   <si>
-    <t>Size</t>
-  </si>
-  <si>
     <t>Data Type</t>
   </si>
   <si>
@@ -82,15 +79,6 @@
   </si>
   <si>
     <t>Name of Restaurant</t>
-  </si>
-  <si>
-    <t>Product_Name</t>
-  </si>
-  <si>
-    <t>Price</t>
-  </si>
-  <si>
-    <t>Price in HUF</t>
   </si>
   <si>
     <t xml:space="preserve">No of customer ratings </t>
@@ -209,16 +197,22 @@
     <t>Full address of restaurant inlcuding street,district,region, postal code, and city</t>
   </si>
   <si>
-    <t>Size of Pizza in cm or Beverage in l</t>
-  </si>
-  <si>
-    <t>Name of Pizza/Beverage</t>
-  </si>
-  <si>
     <t>Tags</t>
   </si>
   <si>
     <t xml:space="preserve">Concatenated string with max 5 tags available for a restaurant </t>
+  </si>
+  <si>
+    <t>margherita_pizza_price</t>
+  </si>
+  <si>
+    <t>beverage_price</t>
+  </si>
+  <si>
+    <t>Price of 32cm Margherita pizza in HUF</t>
+  </si>
+  <si>
+    <t>Price of 0.5 liter beverage in HUF (only Pepsi and Coca-Cola)</t>
   </si>
 </sst>
 </file>
@@ -600,11 +594,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C95F57A2-06DD-4A37-A692-527DC5148D7D}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -618,10 +610,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -632,29 +624,29 @@
         <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="B4" t="s">
         <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -665,7 +657,7 @@
         <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -676,7 +668,7 @@
         <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -687,7 +679,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -698,7 +690,7 @@
         <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -709,7 +701,7 @@
         <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -720,7 +712,7 @@
         <v>13</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -731,7 +723,7 @@
         <v>13</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -742,7 +734,7 @@
         <v>13</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -753,7 +745,7 @@
         <v>13</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -764,7 +756,7 @@
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -775,29 +767,18 @@
         <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="B16" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C16" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>35</v>
-      </c>
-      <c r="B17" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refact file dir + chg readme,variables + rename webscraper
</commit_message>
<xml_diff>
--- a/group_g_assignments/data/clean/Variables.xlsx
+++ b/group_g_assignments/data/clean/Variables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\T450s\Desktop\programming\git\ba_da1\group_g_assignments\data\clean\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/utassydv/Documents/workspaces/other/ba_da1/group_g_assignments/data/clean/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76895433-BA48-41FB-A908-DE9332A1EFC2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6BC3805-15F4-6342-9F96-9AABAF273965}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{BF0F722A-D5EF-4B24-BABF-EC1503209A71}"/>
+    <workbookView xWindow="3940" yWindow="-17480" windowWidth="24240" windowHeight="13140" xr2:uid="{BF0F722A-D5EF-4B24-BABF-EC1503209A71}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,45 +25,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="31">
   <si>
     <t>Variable</t>
-  </si>
-  <si>
-    <t>Restaurant</t>
-  </si>
-  <si>
-    <t>User-Rating</t>
-  </si>
-  <si>
-    <t>No-Ratings</t>
-  </si>
-  <si>
-    <t>Address</t>
-  </si>
-  <si>
-    <t>City</t>
-  </si>
-  <si>
-    <t>Location</t>
-  </si>
-  <si>
-    <t>RestaurantLatitude</t>
-  </si>
-  <si>
-    <t>RestaurantLongitude</t>
-  </si>
-  <si>
-    <t>CenterLatitude</t>
-  </si>
-  <si>
-    <t>CenterLongitude</t>
-  </si>
-  <si>
-    <t>DistanceCityCenter</t>
-  </si>
-  <si>
-    <t>DistanceCEU</t>
   </si>
   <si>
     <t>num</t>
@@ -194,15 +158,6 @@
     <t>City in which the restaurant is located</t>
   </si>
   <si>
-    <t>Full address of restaurant inlcuding street,district,region, postal code, and city</t>
-  </si>
-  <si>
-    <t>Tags</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Concatenated string with max 5 tags available for a restaurant </t>
-  </si>
-  <si>
     <t>margherita_pizza_price</t>
   </si>
   <si>
@@ -213,6 +168,39 @@
   </si>
   <si>
     <t>Price of 0.5 liter beverage in HUF (only Pepsi and Coca-Cola)</t>
+  </si>
+  <si>
+    <t>restaurant</t>
+  </si>
+  <si>
+    <t>user_rating</t>
+  </si>
+  <si>
+    <t>no_ratings</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>restaurant_latitude</t>
+  </si>
+  <si>
+    <t>restaurant_longitude</t>
+  </si>
+  <si>
+    <t>center_latitude</t>
+  </si>
+  <si>
+    <t>center_longitude</t>
+  </si>
+  <si>
+    <t>distance_city_center</t>
+  </si>
+  <si>
+    <t>distance_ceu</t>
   </si>
 </sst>
 </file>
@@ -594,191 +582,171 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C95F57A2-06DD-4A37-A692-527DC5148D7D}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" customWidth="1"/>
-    <col min="3" max="3" width="104.28515625" customWidth="1"/>
+    <col min="1" max="1" width="19.83203125" customWidth="1"/>
+    <col min="2" max="2" width="10.5" customWidth="1"/>
+    <col min="3" max="3" width="104.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B3" t="s">
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" t="s">
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="B11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="B12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
         <v>7</v>
-      </c>
-      <c r="B10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>12</v>
-      </c>
-      <c r="B15" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>29</v>
-      </c>
-      <c r="B16" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16" t="s">
-        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>